<commit_message>
Updated gitignore and removed generated files, also modified some test files
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/TestData.xlsx
+++ b/src/test/resources/testdata/TestData.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amd70\IdeaProjects\OrangeHRMAutomation\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8E4A3F7-D45A-4DDD-8C3E-66B59EC3B410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A6B566F-90DD-4AD0-8BDE-E056178946D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2940" yWindow="3444" windowWidth="17280" windowHeight="8796" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="validLoginData" sheetId="1" r:id="rId1"/>
     <sheet name="inValidLoginData" sheetId="2" r:id="rId2"/>
+    <sheet name="adminUserData" sheetId="3" r:id="rId3"/>
+    <sheet name="AdduserData" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
   <si>
     <t>username</t>
   </si>
@@ -41,16 +43,80 @@
   </si>
   <si>
     <t>Aadmin2468</t>
+  </si>
+  <si>
+    <t>empName</t>
+  </si>
+  <si>
+    <t>BaseUsername</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>amd</t>
+  </si>
+  <si>
+    <t>Login@123</t>
+  </si>
+  <si>
+    <t>Amol</t>
+  </si>
+  <si>
+    <t>firstName</t>
+  </si>
+  <si>
+    <t>middleName</t>
+  </si>
+  <si>
+    <t>lastName</t>
+  </si>
+  <si>
+    <t>confirmPassword</t>
+  </si>
+  <si>
+    <t>empID</t>
+  </si>
+  <si>
+    <t>userName</t>
+  </si>
+  <si>
+    <t>john</t>
+  </si>
+  <si>
+    <t>banega</t>
+  </si>
+  <si>
+    <t>don</t>
+  </si>
+  <si>
+    <t>johndon</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -73,13 +139,31 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -391,8 +475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDE93D20-0043-40A4-91CB-23B30A6EBE52}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -419,4 +503,120 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A1A6467-4B7B-441B-A480-8BC898E8CDBF}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{433921BD-00D0-4ABD-A9A3-F7B44730F4BE}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBF8D793-B4E6-4930-8F52-1A86DB48A3CE}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="6">
+        <v>1700</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{28EB3E14-9431-448E-9D1C-A1B21EB4EBB0}"/>
+    <hyperlink ref="G2" r:id="rId2" xr:uid="{11EA8F8E-BB96-4EE1-9544-D5CA32915F28}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Stabalized framework: Fixed ActionDriver integration, Excel numeric handling, improved validations
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/TestData.xlsx
+++ b/src/test/resources/testdata/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amd70\IdeaProjects\OrangeHRMAutomation\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A6B566F-90DD-4AD0-8BDE-E056178946D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1BFFAED-445A-48E1-8752-1D2CE7CA06AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2940" yWindow="3444" windowWidth="17280" windowHeight="8796" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2940" yWindow="3444" windowWidth="16872" windowHeight="8796" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="validLoginData" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
   <si>
     <t>username</t>
   </si>
@@ -81,16 +81,13 @@
     <t>userName</t>
   </si>
   <si>
-    <t>john</t>
-  </si>
-  <si>
-    <t>banega</t>
-  </si>
-  <si>
-    <t>don</t>
-  </si>
-  <si>
-    <t>johndon</t>
+    <t>kala</t>
+  </si>
+  <si>
+    <t xml:space="preserve">khatta </t>
+  </si>
+  <si>
+    <t>jamun</t>
   </si>
 </sst>
 </file>
@@ -555,7 +552,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -600,10 +597,10 @@
         <v>19</v>
       </c>
       <c r="D2" s="6">
-        <v>1700</v>
+        <v>104</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>9</v>

</xml_diff>